<commit_message>
SIAMv4 - some bugfixing and minor updates
</commit_message>
<xml_diff>
--- a/SIAMv4/SIAMv4_testpop.xlsx
+++ b/SIAMv4/SIAMv4_testpop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA692680-292E-4DB3-B645-19A01380F301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C06686-2EAD-451B-82B8-317EEA557631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Organization</t>
   </si>
@@ -274,13 +274,40 @@
   </si>
   <si>
     <t>accUID~</t>
+  </si>
+  <si>
+    <t>[Actors]</t>
+  </si>
+  <si>
+    <t>actorRef</t>
+  </si>
+  <si>
+    <t>isOwnedBy</t>
+  </si>
+  <si>
+    <t>ownerRef</t>
+  </si>
+  <si>
+    <t>ActorRef</t>
+  </si>
+  <si>
+    <t>PartyRef</t>
+  </si>
+  <si>
+    <t>digid-server</t>
+  </si>
+  <si>
+    <t>Overheid</t>
+  </si>
+  <si>
+    <t>Staat der Nederlanden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,8 +358,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +381,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -383,14 +422,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -426,10 +466,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Linked Cell" xfId="4" builtinId="24"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,377 +952,454 @@
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
-        <f t="shared" ref="A11" si="1">IF($B11="","",CONCATENATE("Org_",$B11))</f>
+        <f>IF($B11="","",CONCATENATE("Org_",$B11))</f>
+        <v>Org_Overheid</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="str">
+        <f t="shared" ref="A12" si="1">IF($B12="","",CONCATENATE("Org_",$B12))</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="5" t="str">
-        <f>IF((ROWS($F$14:$F$17)-COUNTBLANK($F$14:$F$17))=0,"","accAutoLoginReq")</f>
-        <v>accAutoLoginReq</v>
-      </c>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="str">
+        <f>IF($B15="","",CONCATENATE("Actor_",$B15))</f>
+        <v>Actor_digid-server</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="13" t="str">
+        <f>$A11</f>
+        <v>Org_Overheid</v>
+      </c>
+      <c r="D15" s="13" t="str">
+        <f>$B11</f>
+        <v>Overheid</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="str">
+        <f>IF($B16="","",CONCATENATE("Actor_",$B16))</f>
+        <v/>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="13" t="str">
+        <f>$A12</f>
+        <v/>
+      </c>
+      <c r="D16" s="13">
+        <f>$B12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="5" t="str">
+        <f>IF((ROWS($F$19:$F$22)-COUNTBLANK($F$19:$F$22))=0,"","accAutoLoginReq")</f>
+        <v>accAutoLoginReq</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="2" t="str">
-        <f>$A13</f>
+      <c r="F18" s="2" t="str">
+        <f>$A18</f>
         <v>Account</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="13" t="str">
+      <c r="D19" s="13" t="str">
         <f>$A3</f>
         <v>Prs_AdMinderbrood</v>
       </c>
-      <c r="E14" s="13" t="str">
-        <f>$A$10</f>
-        <v>Org_TNO</v>
-      </c>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="E19" s="13" t="str">
+        <f>$A$11</f>
+        <v>Org_Overheid</v>
+      </c>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="13" t="str">
-        <f t="shared" ref="D15" si="2">$A4</f>
+      <c r="D20" s="13" t="str">
+        <f t="shared" ref="D20" si="2">$A4</f>
         <v>Prs_RieksJoosten</v>
       </c>
-      <c r="E15" s="13" t="str">
-        <f t="shared" ref="E15:E16" si="3">$A$10</f>
-        <v>Org_TNO</v>
-      </c>
-      <c r="F15" s="13" t="str">
-        <f>A15</f>
+      <c r="E20" s="13" t="str">
+        <f t="shared" ref="E20:E21" si="3">$A$11</f>
+        <v>Org_Overheid</v>
+      </c>
+      <c r="F20" s="13" t="str">
+        <f>A20</f>
         <v>Acc_TNO_rieks</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+    <row r="21" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="13" t="str">
-        <f t="shared" ref="D16" si="4">$A5</f>
+      <c r="D21" s="13" t="str">
+        <f t="shared" ref="D21" si="4">$A5</f>
         <v>Prs_MichielStornebrink</v>
       </c>
-      <c r="E16" s="13" t="str">
+      <c r="E21" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>Org_TNO</v>
-      </c>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+        <v>Org_Overheid</v>
+      </c>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="13" t="str">
+      <c r="D22" s="13" t="str">
         <f>$A$4</f>
         <v>Prs_RieksJoosten</v>
       </c>
-      <c r="E17" s="13" t="str">
+      <c r="E22" s="13" t="str">
         <f>$A$4</f>
         <v>Prs_RieksJoosten</v>
       </c>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="str">
-        <f t="shared" ref="A18" si="5">IF($B18="","",CONCATENATE("Acc_",$E18,"_",$B18))</f>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="str">
+        <f t="shared" ref="A23" si="5">IF($B23="","",CONCATENATE("Acc_",$E23,"_",$B23))</f>
         <v/>
       </c>
-      <c r="D18" s="13" t="str">
+      <c r="D23" s="13" t="str">
         <f>$A7</f>
         <v/>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="str">
-        <f>$A14</f>
+    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="str">
+        <f>$A19</f>
         <v>Acc_TNO_ad</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="str">
-        <f>$A15</f>
+    <row r="27" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="str">
+        <f>$A20</f>
         <v>Acc_TNO_rieks</v>
       </c>
-      <c r="B22" s="3" t="str">
-        <f>$A15</f>
+      <c r="B27" s="3" t="str">
+        <f>$A20</f>
         <v>Acc_TNO_rieks</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="str">
-        <f>$A16</f>
+    <row r="28" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="str">
+        <f>$A21</f>
         <v>Acc_TNO_michiel</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="str">
-        <f>$A17</f>
+    <row r="29" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="str">
+        <f>$A22</f>
         <v>Acc_Persoonlijk_rieksj</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="str">
-        <f>$A18</f>
+    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14" t="str">
+        <f>$A23</f>
         <v/>
       </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B31" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="12" t="str">
-        <f>$A$16</f>
+      <c r="D33" s="12" t="str">
+        <f>$A$21</f>
         <v>Acc_TNO_michiel</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
+    <row r="34" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="12" t="str">
-        <f t="shared" ref="D29:D30" si="6">$A$16</f>
+      <c r="D34" s="12" t="str">
+        <f t="shared" ref="D34:D35" si="6">$A$21</f>
         <v>Acc_TNO_michiel</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+    <row r="35" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="12" t="str">
+      <c r="D35" s="12" t="str">
         <f t="shared" si="6"/>
         <v>Acc_TNO_michiel</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+    <row r="36" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="12" t="str">
-        <f>$A$22</f>
+      <c r="D36" s="12" t="str">
+        <f>$A$27</f>
         <v>Acc_TNO_rieks</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
+    <row r="37" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="12" t="str">
-        <f>$A$24</f>
+      <c r="D37" s="12" t="str">
+        <f>$A$29</f>
         <v>Acc_Persoonlijk_rieksj</v>
       </c>
     </row>
-    <row r="33" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A31" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A34" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A35" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A36" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A37" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>